<commit_message>
a ver SI FUNCIONA
</commit_message>
<xml_diff>
--- a/Backend/precios_colchones.xlsx
+++ b/Backend/precios_colchones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="393">
   <si>
     <t>Almohada Venecia 0.65 Inducol 1 UN</t>
   </si>
@@ -1100,36 +1100,6 @@
     <t>INDUCOL</t>
   </si>
   <si>
-    <t>[601350] Juego de Cocina DAEWOO 7 Pzas (ø24,20,18 y sarten ø24) Antiadherente DWL-SET7</t>
-  </si>
-  <si>
-    <t>[602241] Juego de Cocina DAEWOO 5 Pzas (ø24,16 y sarten ø24)  Antiadherente DWL-SET5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[600145] Jgo. Cub DYNAMIC TRAMONTINA (6Cuch+6Ten)Mango Madera (22399/030)x 12 </t>
-  </si>
-  <si>
-    <t>[602535] Cubiertos Acero Inox  Juego BUZIOS Tramontina x 24 Pzas(23799)</t>
-  </si>
-  <si>
-    <t>[602410] Cafetera WhitenBlack  c/ filtro removible 1.5L 1000W (WBACWBA02)</t>
-  </si>
-  <si>
-    <t>[602528] Pava Elect ATMA PE1821AP2 1,7 lt -Selec Temp</t>
-  </si>
-  <si>
-    <t>[601890] Sandwichera SMARTLIFE electrica SL-SW3383</t>
-  </si>
-  <si>
-    <t>[601882] Batidora de mano SMARTLIFE SL-HM1035 (PN)</t>
-  </si>
-  <si>
-    <t>[602117] Batidora LILIANA c/ Bowl "Giramix" 450 W ( AAB102 )</t>
-  </si>
-  <si>
-    <t>[601194] Exprimidor de Citricos OSTER SL-JC3400</t>
-  </si>
-  <si>
     <t>DAEWOO</t>
   </si>
   <si>
@@ -1173,15 +1143,74 @@
   </si>
   <si>
     <t>Exprimidor</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/XDWGCE1.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/bHqFsZL.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/BnlMvvZ.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xoOeXeB.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/fDqC38C.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Ni2qK7S.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/HEzen2o.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/okMRIfQ.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Hvk83BU.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xowccjO.png</t>
+  </si>
+  <si>
+    <t>Juego de Cocina DAEWOO 7 Pzas (ø24,20,18 y sarten ø24) Antiadherente DWL-SET7</t>
+  </si>
+  <si>
+    <t>Juego de Cocina DAEWOO 5 Pzas (ø24,16 y sarten ø24)  Antiadherente DWL-SET5</t>
+  </si>
+  <si>
+    <t>Jgo. Cub DYNAMIC TRAMONTINA (6Cuch+6Ten)Mango Madera (22399/030)x 12</t>
+  </si>
+  <si>
+    <t>Cubiertos Acero Inox  Juego BUZIOS Tramontina x 24 Pzas(23799)</t>
+  </si>
+  <si>
+    <t>Cafetera WhitenBlack  c/ filtro removible 1.5L 1000W (WBACWBA02)</t>
+  </si>
+  <si>
+    <t>Pava Elect ATMA PE1821AP2 1,7 lt -Selec Temp</t>
+  </si>
+  <si>
+    <t>Sandwichera SMARTLIFE electrica SL-SW3383</t>
+  </si>
+  <si>
+    <t>Batidora de mano SMARTLIFE SL-HM1035 (PN)</t>
+  </si>
+  <si>
+    <t>Batidora LILIANA c/ Bowl "Giramix" 450 W ( AAB102 )</t>
+  </si>
+  <si>
+    <t>Exprimidor de Citricos OSTER SL-JC3400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1258,7 +1287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1557,15 +1586,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:F350"/>
+  <dimension ref="A1:I350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
-      <selection activeCell="A341" sqref="A341"/>
+    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
+      <selection activeCell="A342" sqref="A342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -7306,7 +7335,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>335</v>
       </c>
@@ -7323,7 +7352,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>336</v>
       </c>
@@ -7340,7 +7369,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>337</v>
       </c>
@@ -7357,7 +7386,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>338</v>
       </c>
@@ -7374,205 +7403,215 @@
         <v>348</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A341" s="3" t="s">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A341" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B341" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="B341" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="C341" s="10">
         <v>89782</v>
       </c>
       <c r="D341" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="E341" t="s">
         <v>349</v>
       </c>
       <c r="F341" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A342" s="3" t="s">
-        <v>359</v>
+        <v>373</v>
+      </c>
+      <c r="I341" s="3"/>
+    </row>
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A342" s="8" t="s">
+        <v>384</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="C342" s="10">
         <v>74536</v>
       </c>
       <c r="D342" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="E342" t="s">
         <v>349</v>
       </c>
       <c r="F342" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A343" s="3" t="s">
-        <v>360</v>
+        <v>374</v>
+      </c>
+      <c r="I342" s="3"/>
+    </row>
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A343" s="8" t="s">
+        <v>385</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="C343" s="10">
         <v>50820</v>
       </c>
       <c r="D343" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="E343" t="s">
         <v>349</v>
       </c>
       <c r="F343" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A344" s="3" t="s">
-        <v>361</v>
+        <v>375</v>
+      </c>
+      <c r="I343" s="3"/>
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A344" s="8" t="s">
+        <v>386</v>
       </c>
       <c r="B344" s="5" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="C344" s="10">
         <v>37268</v>
       </c>
       <c r="D344" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="E344" t="s">
         <v>349</v>
       </c>
       <c r="F344" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A345" s="4" t="s">
-        <v>362</v>
+        <v>376</v>
+      </c>
+      <c r="I344" s="3"/>
+    </row>
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A345" s="8" t="s">
+        <v>387</v>
       </c>
       <c r="B345" s="5" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="C345" s="10">
         <v>42000</v>
       </c>
       <c r="D345" s="8" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="E345" t="s">
         <v>349</v>
       </c>
       <c r="F345" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A346" s="3" t="s">
-        <v>363</v>
+        <v>377</v>
+      </c>
+      <c r="I345" s="4"/>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A346" s="8" t="s">
+        <v>388</v>
       </c>
       <c r="B346" s="5" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C346" s="10">
         <v>45738</v>
       </c>
       <c r="D346" s="8" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="E346" t="s">
         <v>349</v>
       </c>
       <c r="F346" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A347" s="3" t="s">
-        <v>364</v>
+        <v>378</v>
+      </c>
+      <c r="I346" s="3"/>
+    </row>
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A347" s="8" t="s">
+        <v>389</v>
       </c>
       <c r="B347" s="5" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C347" s="10">
         <v>45738</v>
       </c>
       <c r="D347" s="8" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="E347" t="s">
         <v>349</v>
       </c>
       <c r="F347" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A348" s="3" t="s">
-        <v>365</v>
+        <v>379</v>
+      </c>
+      <c r="I347" s="3"/>
+    </row>
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A348" s="8" t="s">
+        <v>390</v>
       </c>
       <c r="B348" s="5" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C348" s="10">
         <v>50820</v>
       </c>
       <c r="D348" s="8" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="E348" t="s">
         <v>349</v>
       </c>
       <c r="F348" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A349" s="3" t="s">
-        <v>366</v>
+        <v>380</v>
+      </c>
+      <c r="I348" s="3"/>
+    </row>
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A349" s="8" t="s">
+        <v>391</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="C349" s="10">
         <v>69999</v>
       </c>
       <c r="D349" s="8" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="E349" t="s">
         <v>349</v>
       </c>
       <c r="F349" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A350" s="3" t="s">
-        <v>367</v>
+        <v>381</v>
+      </c>
+      <c r="I349" s="3"/>
+    </row>
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A350" s="8" t="s">
+        <v>392</v>
       </c>
       <c r="B350" s="5" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="C350" s="10">
         <v>34000</v>
       </c>
       <c r="D350" s="8" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="E350" t="s">
         <v>349</v>
       </c>
       <c r="F350" s="8" t="s">
-        <v>354</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="I350" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
a ver SI FUNCIONA 3333
</commit_message>
<xml_diff>
--- a/Backend/precios_colchones.xlsx
+++ b/Backend/precios_colchones.xlsx
@@ -1589,7 +1589,7 @@
   <dimension ref="A1:I350"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
-      <selection activeCell="A342" sqref="A342"/>
+      <selection activeCell="C341" sqref="C341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7411,7 +7411,7 @@
         <v>358</v>
       </c>
       <c r="C341" s="10">
-        <v>89782</v>
+        <v>89799</v>
       </c>
       <c r="D341" t="s">
         <v>366</v>

</xml_diff>